<commit_message>
VBL LOT PROFILING IS DONE-SOME BLANK ROWS ARE DELETED
</commit_message>
<xml_diff>
--- a/LOT_MGMT/RESULT_FILES/VBL_filtered_data.xlsx
+++ b/LOT_MGMT/RESULT_FILES/VBL_filtered_data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
@@ -458,14 +458,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA1467E"/>
-        <bgColor rgb="FF993366"/>
+        <fgColor rgb="FFFFA6A6"/>
+        <bgColor rgb="FFFFAA95"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFA6A6"/>
-        <bgColor rgb="FFFFAA95"/>
+        <fgColor rgb="FFA1467E"/>
+        <bgColor rgb="FF993366"/>
       </patternFill>
     </fill>
   </fills>
@@ -510,7 +510,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="61">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -735,28 +735,24 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="15" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="16" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="16" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="15" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="15" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="15" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="15" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="16" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="16" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="16" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1013,8 +1009,8 @@
   </sheetPr>
   <dimension ref="A1:N1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I5" activeCellId="0" sqref="I5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.453125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1159,37 +1155,93 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" s="5" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="3"/>
-      <c r="M4" s="3"/>
-      <c r="N4" s="3"/>
-    </row>
-    <row r="5" s="5" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="3"/>
-      <c r="M5" s="3"/>
-      <c r="N5" s="3"/>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="G4" s="13" t="n">
+        <v>467.63</v>
+      </c>
+      <c r="H4" s="9" t="n">
+        <v>467.63</v>
+      </c>
+      <c r="I4" s="12" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="J4" s="9" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="K4" s="9" t="n">
+        <v>0.47</v>
+      </c>
+      <c r="L4" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="M4" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="N4" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" s="13" t="n">
+        <v>467.63</v>
+      </c>
+      <c r="H5" s="9" t="n">
+        <v>467.63</v>
+      </c>
+      <c r="I5" s="12" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="J5" s="9" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="K5" s="9" t="n">
+        <v>0.47</v>
+      </c>
+      <c r="L5" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="M5" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="N5" s="6" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="s">
@@ -1208,25 +1260,25 @@
         <v>18</v>
       </c>
       <c r="F6" s="12" t="n">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="G6" s="13" t="n">
-        <v>467.63</v>
-      </c>
-      <c r="H6" s="9" t="n">
-        <v>467.63</v>
+        <v>467.62</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>22</v>
       </c>
       <c r="I6" s="12" t="n">
-        <v>0.33</v>
+        <v>5.33</v>
       </c>
       <c r="J6" s="9" t="n">
-        <v>0.06</v>
+        <v>0.96</v>
       </c>
       <c r="K6" s="9" t="n">
-        <v>0.47</v>
+        <v>7.5</v>
       </c>
       <c r="L6" s="6" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="M6" s="6" t="n">
         <v>0</v>
@@ -1296,25 +1348,25 @@
         <v>18</v>
       </c>
       <c r="F8" s="12" t="n">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="G8" s="13" t="n">
         <v>467.62</v>
       </c>
       <c r="H8" s="9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I8" s="12" t="n">
-        <v>5.33</v>
+        <v>1.67</v>
       </c>
       <c r="J8" s="9" t="n">
-        <v>0.96</v>
+        <v>0.3</v>
       </c>
       <c r="K8" s="9" t="n">
-        <v>7.5</v>
+        <v>2.34</v>
       </c>
       <c r="L8" s="6" t="n">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="M8" s="6" t="n">
         <v>0</v>
@@ -1340,22 +1392,22 @@
         <v>18</v>
       </c>
       <c r="F9" s="12" t="n">
+        <v>3</v>
+      </c>
+      <c r="G9" s="13" t="n">
+        <v>467.62</v>
+      </c>
+      <c r="H9" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="I9" s="12" t="n">
         <v>1</v>
       </c>
-      <c r="G9" s="13" t="n">
-        <v>467.63</v>
-      </c>
-      <c r="H9" s="9" t="n">
-        <v>467.63</v>
-      </c>
-      <c r="I9" s="12" t="n">
-        <v>0.33</v>
-      </c>
       <c r="J9" s="9" t="n">
-        <v>0.06</v>
+        <v>0.18</v>
       </c>
       <c r="K9" s="9" t="n">
-        <v>0.47</v>
+        <v>1.41</v>
       </c>
       <c r="L9" s="6" t="n">
         <v>0</v>
@@ -1384,25 +1436,25 @@
         <v>18</v>
       </c>
       <c r="F10" s="12" t="n">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="G10" s="13" t="n">
         <v>467.62</v>
       </c>
       <c r="H10" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="I10" s="12" t="n">
-        <v>1.67</v>
+        <v>4.67</v>
       </c>
       <c r="J10" s="9" t="n">
-        <v>0.3</v>
+        <v>0.84</v>
       </c>
       <c r="K10" s="9" t="n">
-        <v>2.34</v>
+        <v>6.56</v>
       </c>
       <c r="L10" s="6" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="M10" s="6" t="n">
         <v>0</v>
@@ -1428,22 +1480,22 @@
         <v>18</v>
       </c>
       <c r="F11" s="12" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G11" s="13" t="n">
-        <v>467.62</v>
-      </c>
-      <c r="H11" s="9" t="s">
-        <v>24</v>
+        <v>467.63</v>
+      </c>
+      <c r="H11" s="9" t="n">
+        <v>467.63</v>
       </c>
       <c r="I11" s="12" t="n">
-        <v>1</v>
+        <v>0.33</v>
       </c>
       <c r="J11" s="9" t="n">
-        <v>0.18</v>
+        <v>0.06</v>
       </c>
       <c r="K11" s="9" t="n">
-        <v>1.41</v>
+        <v>0.47</v>
       </c>
       <c r="L11" s="6" t="n">
         <v>0</v>
@@ -1472,22 +1524,22 @@
         <v>18</v>
       </c>
       <c r="F12" s="12" t="n">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="G12" s="13" t="n">
         <v>467.62</v>
       </c>
       <c r="H12" s="9" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="I12" s="12" t="n">
-        <v>4.67</v>
+        <v>5.33</v>
       </c>
       <c r="J12" s="9" t="n">
-        <v>0.84</v>
+        <v>0.96</v>
       </c>
       <c r="K12" s="9" t="n">
-        <v>6.56</v>
+        <v>7.5</v>
       </c>
       <c r="L12" s="6" t="n">
         <v>0.01</v>
@@ -1543,7 +1595,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" s="14" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="6" t="s">
         <v>14</v>
       </c>
@@ -1560,298 +1612,298 @@
         <v>18</v>
       </c>
       <c r="F14" s="12" t="n">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="G14" s="13" t="n">
-        <v>467.62</v>
-      </c>
-      <c r="H14" s="9" t="s">
-        <v>22</v>
+        <v>467.63</v>
+      </c>
+      <c r="H14" s="9" t="n">
+        <v>467.63</v>
       </c>
       <c r="I14" s="12" t="n">
-        <v>5.33</v>
+        <v>0.33</v>
       </c>
       <c r="J14" s="9" t="n">
-        <v>0.96</v>
+        <v>0.06</v>
       </c>
       <c r="K14" s="9" t="n">
-        <v>7.5</v>
+        <v>0.47</v>
       </c>
       <c r="L14" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="M14" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="N14" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="F15" s="15" t="n">
+        <v>30</v>
+      </c>
+      <c r="G15" s="13" t="n">
+        <v>453.32</v>
+      </c>
+      <c r="H15" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="I15" s="15" t="n">
+        <v>20</v>
+      </c>
+      <c r="J15" s="13" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="K15" s="13" t="n">
+        <v>13.56</v>
+      </c>
+      <c r="L15" s="15" t="n">
+        <v>2.04</v>
+      </c>
+      <c r="M15" s="15" t="n">
+        <v>337</v>
+      </c>
+      <c r="N15" s="15" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" s="16" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="F16" s="15" t="n">
+        <v>30</v>
+      </c>
+      <c r="G16" s="13" t="n">
+        <v>463.33</v>
+      </c>
+      <c r="H16" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="I16" s="15" t="n">
+        <v>20</v>
+      </c>
+      <c r="J16" s="13" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="K16" s="13" t="n">
+        <v>13.86</v>
+      </c>
+      <c r="L16" s="15" t="n">
+        <v>2.09</v>
+      </c>
+      <c r="M16" s="15" t="n">
+        <v>334</v>
+      </c>
+      <c r="N16" s="15" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E17" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="F17" s="14" t="n">
+        <v>6</v>
+      </c>
+      <c r="G17" s="8" t="n">
+        <v>468.88</v>
+      </c>
+      <c r="H17" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="I17" s="14" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="J17" s="8" t="n">
+        <v>0.44</v>
+      </c>
+      <c r="K17" s="8" t="n">
+        <v>2.81</v>
+      </c>
+      <c r="L17" s="14" t="n">
+        <v>0.42</v>
+      </c>
+      <c r="M17" s="14" t="n">
+        <v>331</v>
+      </c>
+      <c r="N17" s="14" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E18" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="F18" s="14" t="n">
+        <v>44</v>
+      </c>
+      <c r="G18" s="8" t="n">
+        <v>468.88</v>
+      </c>
+      <c r="H18" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="I18" s="14" t="n">
+        <v>17.6</v>
+      </c>
+      <c r="J18" s="8" t="n">
+        <v>3.16</v>
+      </c>
+      <c r="K18" s="8" t="n">
+        <v>20.59</v>
+      </c>
+      <c r="L18" s="14" t="n">
+        <v>3.11</v>
+      </c>
+      <c r="M18" s="14" t="n">
+        <v>331</v>
+      </c>
+      <c r="N18" s="14" t="n">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F19" s="17" t="n">
+        <v>20</v>
+      </c>
+      <c r="G19" s="18" t="n">
+        <v>482.65</v>
+      </c>
+      <c r="H19" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="I19" s="17" t="n">
+        <v>3.64</v>
+      </c>
+      <c r="J19" s="9" t="n">
+        <v>0.66</v>
+      </c>
+      <c r="K19" s="9" t="n">
+        <v>2.41</v>
+      </c>
+      <c r="L19" s="6" t="n">
         <v>0.01</v>
       </c>
-      <c r="M14" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="N14" s="6" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F15" s="12" t="n">
-        <v>1</v>
-      </c>
-      <c r="G15" s="13" t="n">
-        <v>467.63</v>
-      </c>
-      <c r="H15" s="9" t="n">
-        <v>467.63</v>
-      </c>
-      <c r="I15" s="12" t="n">
-        <v>0.33</v>
-      </c>
-      <c r="J15" s="9" t="n">
-        <v>0.06</v>
-      </c>
-      <c r="K15" s="9" t="n">
-        <v>0.47</v>
-      </c>
-      <c r="L15" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="M15" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="N15" s="6" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" s="14" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F16" s="12" t="n">
-        <v>1</v>
-      </c>
-      <c r="G16" s="13" t="n">
-        <v>467.63</v>
-      </c>
-      <c r="H16" s="9" t="n">
-        <v>467.63</v>
-      </c>
-      <c r="I16" s="12" t="n">
-        <v>0.33</v>
-      </c>
-      <c r="J16" s="9" t="n">
-        <v>0.06</v>
-      </c>
-      <c r="K16" s="9" t="n">
-        <v>0.47</v>
-      </c>
-      <c r="L16" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="M16" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="N16" s="6" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="B17" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="C17" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="D17" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="E17" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="F17" s="15" t="n">
-        <v>30</v>
-      </c>
-      <c r="G17" s="13" t="n">
-        <v>453.32</v>
-      </c>
-      <c r="H17" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="I17" s="15" t="n">
-        <v>20</v>
-      </c>
-      <c r="J17" s="13" t="n">
-        <v>3.6</v>
-      </c>
-      <c r="K17" s="13" t="n">
-        <v>13.56</v>
-      </c>
-      <c r="L17" s="15" t="n">
-        <v>2.04</v>
-      </c>
-      <c r="M17" s="15" t="n">
-        <v>337</v>
-      </c>
-      <c r="N17" s="15" t="n">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18" s="16" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="B18" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="C18" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="D18" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="E18" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="F18" s="15" t="n">
-        <v>30</v>
-      </c>
-      <c r="G18" s="13" t="n">
-        <v>463.33</v>
-      </c>
-      <c r="H18" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="I18" s="15" t="n">
-        <v>20</v>
-      </c>
-      <c r="J18" s="13" t="n">
-        <v>3.6</v>
-      </c>
-      <c r="K18" s="13" t="n">
-        <v>13.86</v>
-      </c>
-      <c r="L18" s="15" t="n">
-        <v>2.09</v>
-      </c>
-      <c r="M18" s="15" t="n">
-        <v>334</v>
-      </c>
-      <c r="N18" s="15" t="n">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="B19" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="C19" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="D19" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="E19" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="F19" s="14" t="n">
-        <v>6</v>
-      </c>
-      <c r="G19" s="8" t="n">
-        <v>468.88</v>
-      </c>
-      <c r="H19" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="I19" s="14" t="n">
-        <v>2.4</v>
-      </c>
-      <c r="J19" s="8" t="n">
-        <v>0.44</v>
-      </c>
-      <c r="K19" s="8" t="n">
-        <v>2.81</v>
-      </c>
-      <c r="L19" s="14" t="n">
-        <v>0.42</v>
-      </c>
-      <c r="M19" s="14" t="n">
-        <v>331</v>
-      </c>
-      <c r="N19" s="14" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="B20" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="C20" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="D20" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="E20" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="F20" s="14" t="n">
-        <v>44</v>
-      </c>
-      <c r="G20" s="8" t="n">
-        <v>468.88</v>
-      </c>
-      <c r="H20" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="I20" s="14" t="n">
-        <v>17.6</v>
-      </c>
-      <c r="J20" s="8" t="n">
-        <v>3.16</v>
-      </c>
-      <c r="K20" s="8" t="n">
-        <v>20.59</v>
-      </c>
-      <c r="L20" s="14" t="n">
-        <v>3.11</v>
-      </c>
-      <c r="M20" s="14" t="n">
-        <v>331</v>
-      </c>
-      <c r="N20" s="14" t="n">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M19" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="N19" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" s="20" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="C20" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="E20" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="F20" s="16" t="n">
+        <v>20</v>
+      </c>
+      <c r="G20" s="19" t="n">
+        <v>479.21</v>
+      </c>
+      <c r="H20" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="I20" s="16" t="n">
+        <v>20</v>
+      </c>
+      <c r="J20" s="19" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="K20" s="19" t="n">
+        <v>0</v>
+      </c>
+      <c r="L20" s="16" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="M20" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="N20" s="16" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" s="20" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="6" t="s">
         <v>14</v>
       </c>
@@ -1868,78 +1920,78 @@
         <v>18</v>
       </c>
       <c r="F21" s="17" t="n">
-        <v>20</v>
+        <v>83</v>
       </c>
       <c r="G21" s="18" t="n">
-        <v>482.65</v>
+        <v>482.29</v>
       </c>
       <c r="H21" s="9" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="I21" s="17" t="n">
-        <v>3.64</v>
+        <v>15.09</v>
       </c>
       <c r="J21" s="9" t="n">
-        <v>0.66</v>
+        <v>2.72</v>
       </c>
       <c r="K21" s="9" t="n">
-        <v>2.41</v>
+        <v>39.99</v>
       </c>
       <c r="L21" s="6" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="M21" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="N21" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F22" s="21" t="n">
+        <v>20</v>
+      </c>
+      <c r="G22" s="19" t="n">
+        <v>477.42</v>
+      </c>
+      <c r="H22" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="I22" s="6" t="n">
+        <v>20</v>
+      </c>
+      <c r="J22" s="9" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="K22" s="9" t="n">
+        <v>9.64</v>
+      </c>
+      <c r="L22" s="6" t="n">
         <v>0.01</v>
       </c>
-      <c r="M21" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="N21" s="6" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" s="20" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="B22" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="C22" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="D22" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="E22" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="F22" s="16" t="n">
-        <v>20</v>
-      </c>
-      <c r="G22" s="19" t="n">
-        <v>479.21</v>
-      </c>
-      <c r="H22" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="I22" s="16" t="n">
-        <v>20</v>
-      </c>
-      <c r="J22" s="19" t="n">
-        <v>3.6</v>
-      </c>
-      <c r="K22" s="19" t="n">
-        <v>0</v>
-      </c>
-      <c r="L22" s="16" t="n">
-        <v>0.3</v>
-      </c>
-      <c r="M22" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="N22" s="16" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" s="20" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M22" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="N22" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="6" t="s">
         <v>14</v>
       </c>
@@ -1956,25 +2008,25 @@
         <v>18</v>
       </c>
       <c r="F23" s="17" t="n">
-        <v>83</v>
+        <v>7</v>
       </c>
       <c r="G23" s="18" t="n">
         <v>482.29</v>
       </c>
       <c r="H23" s="9" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="I23" s="17" t="n">
-        <v>15.09</v>
+        <v>1.27</v>
       </c>
       <c r="J23" s="9" t="n">
-        <v>2.72</v>
+        <v>0.22</v>
       </c>
       <c r="K23" s="9" t="n">
-        <v>39.99</v>
+        <v>3.37</v>
       </c>
       <c r="L23" s="6" t="n">
-        <v>0.04</v>
+        <v>0</v>
       </c>
       <c r="M23" s="6" t="n">
         <v>0</v>
@@ -1983,487 +2035,487 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E24" s="6" t="s">
+    <row r="24" s="20" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="B24" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="C24" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="D24" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="E24" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="F24" s="20" t="n">
+        <v>50</v>
+      </c>
+      <c r="G24" s="18" t="n">
+        <v>471.03</v>
+      </c>
+      <c r="H24" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="I24" s="20" t="n">
+        <v>20</v>
+      </c>
+      <c r="J24" s="18" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="K24" s="18" t="n">
+        <v>23.53</v>
+      </c>
+      <c r="L24" s="20" t="n">
+        <v>3.55</v>
+      </c>
+      <c r="M24" s="20" t="n">
+        <v>329</v>
+      </c>
+      <c r="N24" s="20" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" s="22" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="B25" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="C25" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="D25" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="E25" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="F25" s="20" t="n">
+        <v>20</v>
+      </c>
+      <c r="G25" s="18" t="n">
+        <v>473.74</v>
+      </c>
+      <c r="H25" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="I25" s="20" t="n">
+        <v>20</v>
+      </c>
+      <c r="J25" s="18" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="K25" s="18" t="n">
+        <v>9.41</v>
+      </c>
+      <c r="L25" s="20" t="n">
+        <v>1.43</v>
+      </c>
+      <c r="M25" s="20" t="n">
+        <v>329</v>
+      </c>
+      <c r="N25" s="20" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" s="20" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E26" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="F24" s="21" t="n">
-        <v>20</v>
-      </c>
-      <c r="G24" s="19" t="n">
-        <v>477.42</v>
-      </c>
-      <c r="H24" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="I24" s="6" t="n">
-        <v>20</v>
-      </c>
-      <c r="J24" s="9" t="n">
-        <v>3.6</v>
-      </c>
-      <c r="K24" s="9" t="n">
-        <v>9.64</v>
-      </c>
-      <c r="L24" s="6" t="n">
+      <c r="F26" s="23" t="n">
+        <v>30</v>
+      </c>
+      <c r="G26" s="24" t="n">
+        <v>482.03</v>
+      </c>
+      <c r="H26" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="I26" s="6" t="n">
+        <v>12</v>
+      </c>
+      <c r="J26" s="9" t="n">
+        <v>2.16</v>
+      </c>
+      <c r="K26" s="9" t="n">
+        <v>14.44</v>
+      </c>
+      <c r="L26" s="6" t="n">
         <v>0.01</v>
       </c>
-      <c r="M24" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="N24" s="6" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B25" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D25" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E25" s="6" t="s">
+      <c r="M26" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="N26" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" s="10" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E27" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="F25" s="17" t="n">
-        <v>7</v>
-      </c>
-      <c r="G25" s="18" t="n">
-        <v>482.29</v>
-      </c>
-      <c r="H25" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="I25" s="17" t="n">
-        <v>1.27</v>
-      </c>
-      <c r="J25" s="9" t="n">
-        <v>0.22</v>
-      </c>
-      <c r="K25" s="9" t="n">
-        <v>3.37</v>
-      </c>
-      <c r="L25" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="M25" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="N25" s="6" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" s="20" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="B26" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="C26" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="D26" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="E26" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="F26" s="20" t="n">
+      <c r="F27" s="23" t="n">
+        <v>20</v>
+      </c>
+      <c r="G27" s="24" t="n">
+        <v>482.39</v>
+      </c>
+      <c r="H27" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="I27" s="6" t="n">
+        <v>8</v>
+      </c>
+      <c r="J27" s="9" t="n">
+        <v>1.44</v>
+      </c>
+      <c r="K27" s="9" t="n">
+        <v>2.41</v>
+      </c>
+      <c r="L27" s="6" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="M27" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="N27" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" s="10" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="B28" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="C28" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="D28" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="E28" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="F28" s="20" t="n">
+        <v>20</v>
+      </c>
+      <c r="G28" s="18" t="n">
+        <v>478.21</v>
+      </c>
+      <c r="H28" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="I28" s="20" t="n">
+        <v>20</v>
+      </c>
+      <c r="J28" s="18" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="K28" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="L28" s="20" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="M28" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="N28" s="20" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="B29" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="C29" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="D29" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="E29" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="F29" s="22" t="n">
         <v>50</v>
       </c>
-      <c r="G26" s="18" t="n">
-        <v>471.03</v>
-      </c>
-      <c r="H26" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="I26" s="20" t="n">
-        <v>20</v>
-      </c>
-      <c r="J26" s="18" t="n">
-        <v>3.6</v>
-      </c>
-      <c r="K26" s="18" t="n">
-        <v>23.53</v>
-      </c>
-      <c r="L26" s="20" t="n">
-        <v>3.55</v>
-      </c>
-      <c r="M26" s="20" t="n">
-        <v>329</v>
-      </c>
-      <c r="N26" s="20" t="n">
+      <c r="G29" s="24" t="n">
+        <v>469.03</v>
+      </c>
+      <c r="H29" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="I29" s="22" t="n">
+        <v>20</v>
+      </c>
+      <c r="J29" s="24" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="K29" s="24" t="n">
+        <v>23.4</v>
+      </c>
+      <c r="L29" s="22" t="n">
+        <v>3.53</v>
+      </c>
+      <c r="M29" s="22" t="n">
+        <v>322</v>
+      </c>
+      <c r="N29" s="22" t="n">
         <v>50</v>
       </c>
     </row>
-    <row r="27" s="22" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="B27" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="C27" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="D27" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="E27" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="F27" s="20" t="n">
-        <v>20</v>
-      </c>
-      <c r="G27" s="18" t="n">
-        <v>473.74</v>
-      </c>
-      <c r="H27" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="I27" s="20" t="n">
-        <v>20</v>
-      </c>
-      <c r="J27" s="18" t="n">
-        <v>3.6</v>
-      </c>
-      <c r="K27" s="18" t="n">
-        <v>9.41</v>
-      </c>
-      <c r="L27" s="20" t="n">
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="B30" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="C30" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="D30" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="E30" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="F30" s="20" t="n">
+        <v>20</v>
+      </c>
+      <c r="G30" s="25" t="n">
+        <v>474.64</v>
+      </c>
+      <c r="H30" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="I30" s="20" t="n">
+        <v>20</v>
+      </c>
+      <c r="J30" s="25" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="K30" s="25" t="n">
+        <v>9.46</v>
+      </c>
+      <c r="L30" s="20" t="n">
         <v>1.43</v>
       </c>
-      <c r="M27" s="20" t="n">
-        <v>329</v>
-      </c>
-      <c r="N27" s="20" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="28" s="20" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B28" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="C28" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D28" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E28" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F28" s="23" t="n">
+      <c r="M30" s="20" t="n">
+        <v>361</v>
+      </c>
+      <c r="N30" s="20" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="B31" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="C31" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="D31" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="E31" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="F31" s="26" t="n">
+        <v>50</v>
+      </c>
+      <c r="G31" s="27" t="n">
+        <v>483.05</v>
+      </c>
+      <c r="H31" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="I31" s="26" t="n">
+        <v>20</v>
+      </c>
+      <c r="J31" s="27" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="K31" s="27" t="n">
+        <v>24.3</v>
+      </c>
+      <c r="L31" s="26" t="n">
+        <v>3.64</v>
+      </c>
+      <c r="M31" s="26" t="n">
+        <v>359</v>
+      </c>
+      <c r="N31" s="26" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="B32" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="C32" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="D32" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="E32" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="F32" s="26" t="n">
+        <v>20</v>
+      </c>
+      <c r="G32" s="27" t="n">
+        <v>488.36</v>
+      </c>
+      <c r="H32" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="I32" s="26" t="n">
+        <v>13.33</v>
+      </c>
+      <c r="J32" s="27" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="K32" s="27" t="n">
+        <v>14.58</v>
+      </c>
+      <c r="L32" s="26" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="M32" s="26" t="n">
+        <v>359</v>
+      </c>
+      <c r="N32" s="26" t="n">
         <v>30</v>
       </c>
-      <c r="G28" s="24" t="n">
-        <v>482.03</v>
-      </c>
-      <c r="H28" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="I28" s="6" t="n">
-        <v>12</v>
-      </c>
-      <c r="J28" s="9" t="n">
-        <v>2.16</v>
-      </c>
-      <c r="K28" s="9" t="n">
-        <v>14.44</v>
-      </c>
-      <c r="L28" s="6" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="M28" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="N28" s="6" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" s="10" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B29" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="C29" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D29" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E29" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F29" s="23" t="n">
-        <v>20</v>
-      </c>
-      <c r="G29" s="24" t="n">
-        <v>482.39</v>
-      </c>
-      <c r="H29" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="I29" s="6" t="n">
-        <v>8</v>
-      </c>
-      <c r="J29" s="9" t="n">
-        <v>1.44</v>
-      </c>
-      <c r="K29" s="9" t="n">
-        <v>2.41</v>
-      </c>
-      <c r="L29" s="6" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="M29" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="N29" s="6" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" s="10" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="B30" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="C30" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="D30" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="E30" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="F30" s="20" t="n">
-        <v>20</v>
-      </c>
-      <c r="G30" s="18" t="n">
-        <v>478.21</v>
-      </c>
-      <c r="H30" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="I30" s="20" t="n">
-        <v>20</v>
-      </c>
-      <c r="J30" s="18" t="n">
-        <v>3.6</v>
-      </c>
-      <c r="K30" s="18" t="n">
-        <v>0</v>
-      </c>
-      <c r="L30" s="20" t="n">
-        <v>0.3</v>
-      </c>
-      <c r="M30" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="N30" s="20" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="B31" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="C31" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="D31" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="E31" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="F31" s="22" t="n">
-        <v>50</v>
-      </c>
-      <c r="G31" s="24" t="n">
-        <v>469.03</v>
-      </c>
-      <c r="H31" s="24" t="s">
-        <v>48</v>
-      </c>
-      <c r="I31" s="22" t="n">
-        <v>20</v>
-      </c>
-      <c r="J31" s="24" t="n">
-        <v>3.6</v>
-      </c>
-      <c r="K31" s="24" t="n">
-        <v>23.4</v>
-      </c>
-      <c r="L31" s="22" t="n">
-        <v>3.53</v>
-      </c>
-      <c r="M31" s="22" t="n">
-        <v>322</v>
-      </c>
-      <c r="N31" s="22" t="n">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="B32" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="C32" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="D32" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="E32" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="F32" s="20" t="n">
-        <v>20</v>
-      </c>
-      <c r="G32" s="25" t="n">
-        <v>474.64</v>
-      </c>
-      <c r="H32" s="25" t="s">
-        <v>50</v>
-      </c>
-      <c r="I32" s="20" t="n">
-        <v>20</v>
-      </c>
-      <c r="J32" s="25" t="n">
-        <v>3.6</v>
-      </c>
-      <c r="K32" s="25" t="n">
-        <v>9.46</v>
-      </c>
-      <c r="L32" s="20" t="n">
-        <v>1.43</v>
-      </c>
-      <c r="M32" s="20" t="n">
-        <v>361</v>
-      </c>
-      <c r="N32" s="20" t="n">
-        <v>20</v>
-      </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="B33" s="26" t="s">
+      <c r="A33" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="B33" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="C33" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="D33" s="26" t="s">
-        <v>17</v>
-      </c>
-      <c r="E33" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="F33" s="26" t="n">
-        <v>50</v>
-      </c>
-      <c r="G33" s="27" t="n">
-        <v>483.05</v>
-      </c>
-      <c r="H33" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="I33" s="26" t="n">
-        <v>20</v>
-      </c>
-      <c r="J33" s="27" t="n">
-        <v>3.6</v>
-      </c>
-      <c r="K33" s="27" t="n">
-        <v>24.3</v>
-      </c>
-      <c r="L33" s="26" t="n">
-        <v>3.64</v>
-      </c>
-      <c r="M33" s="26" t="n">
+      <c r="C33" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="D33" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="E33" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="F33" s="28" t="n">
+        <v>10</v>
+      </c>
+      <c r="G33" s="29" t="n">
+        <v>488.36</v>
+      </c>
+      <c r="H33" s="29" t="s">
+        <v>53</v>
+      </c>
+      <c r="I33" s="28" t="n">
+        <v>6.67</v>
+      </c>
+      <c r="J33" s="29" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="K33" s="29" t="n">
+        <v>14.58</v>
+      </c>
+      <c r="L33" s="28" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="M33" s="28" t="n">
         <v>359</v>
       </c>
-      <c r="N33" s="26" t="n">
-        <v>50</v>
+      <c r="N33" s="28" t="n">
+        <v>30</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="B34" s="26" t="s">
+      <c r="A34" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="B34" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="C34" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="D34" s="26" t="s">
-        <v>17</v>
-      </c>
-      <c r="E34" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="F34" s="26" t="n">
-        <v>20</v>
-      </c>
-      <c r="G34" s="27" t="n">
-        <v>488.36</v>
-      </c>
-      <c r="H34" s="27" t="s">
-        <v>53</v>
-      </c>
-      <c r="I34" s="26" t="n">
-        <v>13.33</v>
-      </c>
-      <c r="J34" s="27" t="n">
-        <v>3.6</v>
-      </c>
-      <c r="K34" s="27" t="n">
+      <c r="C34" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="D34" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="E34" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="F34" s="28" t="n">
+        <v>30</v>
+      </c>
+      <c r="G34" s="29" t="n">
+        <v>493.36</v>
+      </c>
+      <c r="H34" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="I34" s="28" t="n">
+        <v>20</v>
+      </c>
+      <c r="J34" s="29" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="K34" s="29" t="n">
         <v>14.58</v>
       </c>
-      <c r="L34" s="26" t="n">
-        <v>2.2</v>
-      </c>
-      <c r="M34" s="26" t="n">
+      <c r="L34" s="28" t="n">
+        <v>2.22</v>
+      </c>
+      <c r="M34" s="28" t="n">
         <v>359</v>
       </c>
-      <c r="N34" s="26" t="n">
+      <c r="N34" s="28" t="n">
         <v>30</v>
       </c>
     </row>
@@ -2472,7 +2524,7 @@
         <v>14</v>
       </c>
       <c r="B35" s="28" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C35" s="28" t="s">
         <v>16</v>
@@ -2484,31 +2536,31 @@
         <v>27</v>
       </c>
       <c r="F35" s="28" t="n">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="G35" s="29" t="n">
-        <v>488.36</v>
+        <v>499.07</v>
       </c>
       <c r="H35" s="29" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="I35" s="28" t="n">
-        <v>6.67</v>
+        <v>20</v>
       </c>
       <c r="J35" s="29" t="n">
         <v>3.6</v>
       </c>
       <c r="K35" s="29" t="n">
-        <v>14.58</v>
+        <v>25.05</v>
       </c>
       <c r="L35" s="28" t="n">
-        <v>2.2</v>
+        <v>3.76</v>
       </c>
       <c r="M35" s="28" t="n">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="N35" s="28" t="n">
-        <v>30</v>
+        <v>50</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2516,7 +2568,7 @@
         <v>14</v>
       </c>
       <c r="B36" s="28" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C36" s="28" t="s">
         <v>16</v>
@@ -2528,13 +2580,13 @@
         <v>27</v>
       </c>
       <c r="F36" s="28" t="n">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="G36" s="29" t="n">
-        <v>493.36</v>
+        <v>504.97</v>
       </c>
       <c r="H36" s="29" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="I36" s="28" t="n">
         <v>20</v>
@@ -2543,280 +2595,280 @@
         <v>3.6</v>
       </c>
       <c r="K36" s="29" t="n">
-        <v>14.58</v>
+        <v>25.05</v>
       </c>
       <c r="L36" s="28" t="n">
-        <v>2.22</v>
+        <v>3.81</v>
       </c>
       <c r="M36" s="28" t="n">
+        <v>355</v>
+      </c>
+      <c r="N36" s="28" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F37" s="30" t="n">
+        <v>200</v>
+      </c>
+      <c r="G37" s="31" t="n">
+        <v>510.35</v>
+      </c>
+      <c r="H37" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="I37" s="6" t="n">
+        <v>20</v>
+      </c>
+      <c r="J37" s="9" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="K37" s="9" t="n">
+        <v>102.2</v>
+      </c>
+      <c r="L37" s="6" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="M37" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="N37" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="B38" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="C38" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="D38" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="E38" s="32" t="s">
+        <v>27</v>
+      </c>
+      <c r="F38" s="32" t="n">
+        <v>35</v>
+      </c>
+      <c r="G38" s="33" t="n">
+        <v>479.5</v>
+      </c>
+      <c r="H38" s="33" t="s">
+        <v>61</v>
+      </c>
+      <c r="I38" s="32" t="n">
+        <v>14</v>
+      </c>
+      <c r="J38" s="34" t="n">
+        <v>2.52</v>
+      </c>
+      <c r="K38" s="34" t="n">
+        <v>0</v>
+      </c>
+      <c r="L38" s="32" t="n">
+        <v>0.52</v>
+      </c>
+      <c r="M38" s="32" t="n">
+        <v>0</v>
+      </c>
+      <c r="N38" s="32" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="B39" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="C39" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="D39" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="E39" s="32" t="s">
+        <v>27</v>
+      </c>
+      <c r="F39" s="32" t="n">
+        <v>15</v>
+      </c>
+      <c r="G39" s="33" t="n">
+        <v>479.5</v>
+      </c>
+      <c r="H39" s="33" t="s">
+        <v>62</v>
+      </c>
+      <c r="I39" s="32" t="n">
+        <v>6</v>
+      </c>
+      <c r="J39" s="34" t="n">
+        <v>1.08</v>
+      </c>
+      <c r="K39" s="34" t="n">
+        <v>0</v>
+      </c>
+      <c r="L39" s="32" t="n">
+        <v>0.23</v>
+      </c>
+      <c r="M39" s="32" t="n">
+        <v>0</v>
+      </c>
+      <c r="N39" s="32" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E40" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F40" s="35" t="n">
+        <v>50</v>
+      </c>
+      <c r="G40" s="33" t="n">
+        <v>495.39</v>
+      </c>
+      <c r="H40" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="I40" s="6" t="n">
+        <v>20</v>
+      </c>
+      <c r="J40" s="9" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="K40" s="9" t="n">
+        <v>6.09</v>
+      </c>
+      <c r="L40" s="6" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="M40" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="N40" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="B41" s="36" t="s">
+        <v>64</v>
+      </c>
+      <c r="C41" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="D41" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="E41" s="36" t="s">
+        <v>27</v>
+      </c>
+      <c r="F41" s="36" t="n">
+        <v>50</v>
+      </c>
+      <c r="G41" s="31" t="n">
+        <v>498.06</v>
+      </c>
+      <c r="H41" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="I41" s="36" t="n">
+        <v>20</v>
+      </c>
+      <c r="J41" s="37" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="K41" s="37" t="n">
+        <v>24.85</v>
+      </c>
+      <c r="L41" s="36" t="n">
+        <v>3.75</v>
+      </c>
+      <c r="M41" s="36" t="n">
         <v>359</v>
       </c>
-      <c r="N36" s="28" t="n">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="B37" s="28" t="s">
-        <v>55</v>
-      </c>
-      <c r="C37" s="28" t="s">
-        <v>16</v>
-      </c>
-      <c r="D37" s="28" t="s">
-        <v>17</v>
-      </c>
-      <c r="E37" s="28" t="s">
-        <v>27</v>
-      </c>
-      <c r="F37" s="28" t="n">
+      <c r="N41" s="36" t="n">
         <v>50</v>
       </c>
-      <c r="G37" s="29" t="n">
-        <v>499.07</v>
-      </c>
-      <c r="H37" s="29" t="s">
-        <v>56</v>
-      </c>
-      <c r="I37" s="28" t="n">
-        <v>20</v>
-      </c>
-      <c r="J37" s="29" t="n">
-        <v>3.6</v>
-      </c>
-      <c r="K37" s="29" t="n">
-        <v>25.05</v>
-      </c>
-      <c r="L37" s="28" t="n">
-        <v>3.76</v>
-      </c>
-      <c r="M37" s="28" t="n">
-        <v>355</v>
-      </c>
-      <c r="N37" s="28" t="n">
+    </row>
+    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="B42" s="36" t="s">
+        <v>64</v>
+      </c>
+      <c r="C42" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="D42" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="E42" s="36" t="s">
+        <v>27</v>
+      </c>
+      <c r="F42" s="36" t="n">
         <v>50</v>
       </c>
-    </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="B38" s="28" t="s">
-        <v>55</v>
-      </c>
-      <c r="C38" s="28" t="s">
-        <v>16</v>
-      </c>
-      <c r="D38" s="28" t="s">
-        <v>17</v>
-      </c>
-      <c r="E38" s="28" t="s">
-        <v>27</v>
-      </c>
-      <c r="F38" s="28" t="n">
+      <c r="G42" s="31" t="n">
+        <v>493.06</v>
+      </c>
+      <c r="H42" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="I42" s="36" t="n">
+        <v>20</v>
+      </c>
+      <c r="J42" s="37" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="K42" s="37" t="n">
+        <v>24.85</v>
+      </c>
+      <c r="L42" s="36" t="n">
+        <v>3.71</v>
+      </c>
+      <c r="M42" s="36" t="n">
+        <v>359</v>
+      </c>
+      <c r="N42" s="36" t="n">
         <v>50</v>
-      </c>
-      <c r="G38" s="29" t="n">
-        <v>504.97</v>
-      </c>
-      <c r="H38" s="29" t="s">
-        <v>57</v>
-      </c>
-      <c r="I38" s="28" t="n">
-        <v>20</v>
-      </c>
-      <c r="J38" s="29" t="n">
-        <v>3.6</v>
-      </c>
-      <c r="K38" s="29" t="n">
-        <v>25.05</v>
-      </c>
-      <c r="L38" s="28" t="n">
-        <v>3.81</v>
-      </c>
-      <c r="M38" s="28" t="n">
-        <v>355</v>
-      </c>
-      <c r="N38" s="28" t="n">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B39" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="C39" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D39" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E39" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F39" s="30" t="n">
-        <v>200</v>
-      </c>
-      <c r="G39" s="31" t="n">
-        <v>510.35</v>
-      </c>
-      <c r="H39" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="I39" s="6" t="n">
-        <v>20</v>
-      </c>
-      <c r="J39" s="9" t="n">
-        <v>3.6</v>
-      </c>
-      <c r="K39" s="9" t="n">
-        <v>102.2</v>
-      </c>
-      <c r="L39" s="6" t="n">
-        <v>0.12</v>
-      </c>
-      <c r="M39" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="N39" s="6" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="B40" s="32" t="s">
-        <v>60</v>
-      </c>
-      <c r="C40" s="32" t="s">
-        <v>16</v>
-      </c>
-      <c r="D40" s="32" t="s">
-        <v>17</v>
-      </c>
-      <c r="E40" s="32" t="s">
-        <v>27</v>
-      </c>
-      <c r="F40" s="32" t="n">
-        <v>35</v>
-      </c>
-      <c r="G40" s="33" t="n">
-        <v>479.5</v>
-      </c>
-      <c r="H40" s="33" t="s">
-        <v>61</v>
-      </c>
-      <c r="I40" s="32" t="n">
-        <v>14</v>
-      </c>
-      <c r="J40" s="34" t="n">
-        <v>2.52</v>
-      </c>
-      <c r="K40" s="34" t="n">
-        <v>0</v>
-      </c>
-      <c r="L40" s="32" t="n">
-        <v>0.52</v>
-      </c>
-      <c r="M40" s="32" t="n">
-        <v>0</v>
-      </c>
-      <c r="N40" s="32" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="B41" s="32" t="s">
-        <v>60</v>
-      </c>
-      <c r="C41" s="32" t="s">
-        <v>16</v>
-      </c>
-      <c r="D41" s="32" t="s">
-        <v>17</v>
-      </c>
-      <c r="E41" s="32" t="s">
-        <v>27</v>
-      </c>
-      <c r="F41" s="32" t="n">
-        <v>15</v>
-      </c>
-      <c r="G41" s="33" t="n">
-        <v>479.5</v>
-      </c>
-      <c r="H41" s="33" t="s">
-        <v>62</v>
-      </c>
-      <c r="I41" s="32" t="n">
-        <v>6</v>
-      </c>
-      <c r="J41" s="34" t="n">
-        <v>1.08</v>
-      </c>
-      <c r="K41" s="34" t="n">
-        <v>0</v>
-      </c>
-      <c r="L41" s="32" t="n">
-        <v>0.23</v>
-      </c>
-      <c r="M41" s="32" t="n">
-        <v>0</v>
-      </c>
-      <c r="N41" s="32" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B42" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="C42" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D42" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E42" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F42" s="35" t="n">
-        <v>50</v>
-      </c>
-      <c r="G42" s="33" t="n">
-        <v>495.39</v>
-      </c>
-      <c r="H42" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="I42" s="6" t="n">
-        <v>20</v>
-      </c>
-      <c r="J42" s="9" t="n">
-        <v>3.6</v>
-      </c>
-      <c r="K42" s="9" t="n">
-        <v>6.09</v>
-      </c>
-      <c r="L42" s="6" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="M42" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="N42" s="6" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2839,10 +2891,10 @@
         <v>50</v>
       </c>
       <c r="G43" s="31" t="n">
-        <v>498.06</v>
+        <v>503.06</v>
       </c>
       <c r="H43" s="31" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="I43" s="36" t="n">
         <v>20</v>
@@ -2854,13 +2906,13 @@
         <v>24.85</v>
       </c>
       <c r="L43" s="36" t="n">
-        <v>3.75</v>
+        <v>3.8</v>
       </c>
       <c r="M43" s="36" t="n">
         <v>359</v>
       </c>
       <c r="N43" s="36" t="n">
-        <v>50</v>
+        <v>35</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2868,7 +2920,7 @@
         <v>14</v>
       </c>
       <c r="B44" s="36" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="C44" s="36" t="s">
         <v>16</v>
@@ -2883,10 +2935,10 @@
         <v>50</v>
       </c>
       <c r="G44" s="31" t="n">
-        <v>493.06</v>
+        <v>507.07</v>
       </c>
       <c r="H44" s="31" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="I44" s="36" t="n">
         <v>20</v>
@@ -2895,103 +2947,103 @@
         <v>3.6</v>
       </c>
       <c r="K44" s="37" t="n">
-        <v>24.85</v>
+        <v>25.39</v>
       </c>
       <c r="L44" s="36" t="n">
-        <v>3.71</v>
+        <v>3.83</v>
       </c>
       <c r="M44" s="36" t="n">
-        <v>359</v>
+        <v>0</v>
       </c>
       <c r="N44" s="36" t="n">
-        <v>50</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="36" t="s">
-        <v>14</v>
-      </c>
-      <c r="B45" s="36" t="s">
-        <v>64</v>
-      </c>
-      <c r="C45" s="36" t="s">
-        <v>16</v>
-      </c>
-      <c r="D45" s="36" t="s">
-        <v>17</v>
-      </c>
-      <c r="E45" s="36" t="s">
-        <v>27</v>
-      </c>
-      <c r="F45" s="36" t="n">
-        <v>50</v>
-      </c>
-      <c r="G45" s="31" t="n">
-        <v>503.06</v>
-      </c>
-      <c r="H45" s="31" t="s">
-        <v>67</v>
-      </c>
-      <c r="I45" s="36" t="n">
-        <v>20</v>
-      </c>
-      <c r="J45" s="37" t="n">
-        <v>3.6</v>
-      </c>
-      <c r="K45" s="37" t="n">
-        <v>24.85</v>
-      </c>
-      <c r="L45" s="36" t="n">
-        <v>3.8</v>
-      </c>
-      <c r="M45" s="36" t="n">
-        <v>359</v>
-      </c>
-      <c r="N45" s="36" t="n">
-        <v>35</v>
+      <c r="A45" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E45" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F45" s="5" t="n">
+        <v>30</v>
+      </c>
+      <c r="G45" s="38" t="n">
+        <v>512.39</v>
+      </c>
+      <c r="H45" s="38" t="s">
+        <v>70</v>
+      </c>
+      <c r="I45" s="5" t="n">
+        <v>20</v>
+      </c>
+      <c r="J45" s="38" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="K45" s="38" t="n">
+        <v>15.24</v>
+      </c>
+      <c r="L45" s="5" t="n">
+        <v>2.32</v>
+      </c>
+      <c r="M45" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="N45" s="5" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="36" t="s">
-        <v>14</v>
-      </c>
-      <c r="B46" s="36" t="s">
+      <c r="A46" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="B46" s="39" t="s">
         <v>68</v>
       </c>
-      <c r="C46" s="36" t="s">
-        <v>16</v>
-      </c>
-      <c r="D46" s="36" t="s">
-        <v>17</v>
-      </c>
-      <c r="E46" s="36" t="s">
-        <v>27</v>
-      </c>
-      <c r="F46" s="36" t="n">
-        <v>50</v>
-      </c>
-      <c r="G46" s="31" t="n">
-        <v>507.07</v>
-      </c>
-      <c r="H46" s="31" t="s">
-        <v>69</v>
-      </c>
-      <c r="I46" s="36" t="n">
-        <v>20</v>
-      </c>
-      <c r="J46" s="37" t="n">
-        <v>3.6</v>
-      </c>
-      <c r="K46" s="37" t="n">
-        <v>25.39</v>
-      </c>
-      <c r="L46" s="36" t="n">
-        <v>3.83</v>
-      </c>
-      <c r="M46" s="36" t="n">
-        <v>0</v>
-      </c>
-      <c r="N46" s="36" t="n">
+      <c r="C46" s="39" t="s">
+        <v>16</v>
+      </c>
+      <c r="D46" s="39" t="s">
+        <v>17</v>
+      </c>
+      <c r="E46" s="39" t="s">
+        <v>71</v>
+      </c>
+      <c r="F46" s="39" t="n">
+        <v>105</v>
+      </c>
+      <c r="G46" s="40" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="H46" s="40" t="n">
+        <v>52.5</v>
+      </c>
+      <c r="I46" s="39" t="n">
+        <v>0</v>
+      </c>
+      <c r="J46" s="40" t="n">
+        <v>0</v>
+      </c>
+      <c r="K46" s="40" t="n">
+        <v>0</v>
+      </c>
+      <c r="L46" s="39" t="n">
+        <v>0</v>
+      </c>
+      <c r="M46" s="39" t="n">
+        <v>0</v>
+      </c>
+      <c r="N46" s="39" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3000,7 +3052,7 @@
         <v>14</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="C47" s="5" t="s">
         <v>16</v>
@@ -3015,10 +3067,10 @@
         <v>30</v>
       </c>
       <c r="G47" s="38" t="n">
-        <v>512.39</v>
+        <v>517.4</v>
       </c>
       <c r="H47" s="38" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="I47" s="5" t="n">
         <v>20</v>
@@ -3027,10 +3079,10 @@
         <v>3.6</v>
       </c>
       <c r="K47" s="38" t="n">
-        <v>15.24</v>
+        <v>15.48</v>
       </c>
       <c r="L47" s="5" t="n">
-        <v>2.32</v>
+        <v>2.34</v>
       </c>
       <c r="M47" s="5" t="n">
         <v>0</v>
@@ -3040,46 +3092,46 @@
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="39" t="s">
-        <v>14</v>
-      </c>
-      <c r="B48" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="C48" s="39" t="s">
-        <v>16</v>
-      </c>
-      <c r="D48" s="39" t="s">
-        <v>17</v>
-      </c>
-      <c r="E48" s="39" t="s">
-        <v>71</v>
-      </c>
-      <c r="F48" s="39" t="n">
-        <v>105</v>
-      </c>
-      <c r="G48" s="40" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="H48" s="40" t="n">
-        <v>52.5</v>
-      </c>
-      <c r="I48" s="39" t="n">
-        <v>0</v>
-      </c>
-      <c r="J48" s="40" t="n">
-        <v>0</v>
-      </c>
-      <c r="K48" s="40" t="n">
-        <v>0</v>
-      </c>
-      <c r="L48" s="39" t="n">
-        <v>0</v>
-      </c>
-      <c r="M48" s="39" t="n">
-        <v>0</v>
-      </c>
-      <c r="N48" s="39" t="n">
+      <c r="A48" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D48" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E48" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F48" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="G48" s="38" t="n">
+        <v>522.86</v>
+      </c>
+      <c r="H48" s="38" t="s">
+        <v>75</v>
+      </c>
+      <c r="I48" s="5" t="n">
+        <v>20</v>
+      </c>
+      <c r="J48" s="38" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="K48" s="38" t="n">
+        <v>20.87</v>
+      </c>
+      <c r="L48" s="5" t="n">
+        <v>3.15</v>
+      </c>
+      <c r="M48" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="N48" s="5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3088,7 +3140,7 @@
         <v>14</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="C49" s="5" t="s">
         <v>16</v>
@@ -3103,626 +3155,540 @@
         <v>30</v>
       </c>
       <c r="G49" s="38" t="n">
+        <v>526.71</v>
+      </c>
+      <c r="H49" s="38" t="s">
+        <v>77</v>
+      </c>
+      <c r="I49" s="5" t="n">
+        <v>20</v>
+      </c>
+      <c r="J49" s="38" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="K49" s="38" t="n">
+        <v>15.76</v>
+      </c>
+      <c r="L49" s="5" t="n">
+        <v>2.38</v>
+      </c>
+      <c r="M49" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="N49" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B50" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="C50" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D50" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E50" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F50" s="41" t="n">
+        <v>50</v>
+      </c>
+      <c r="G50" s="42" t="n">
+        <v>562.34</v>
+      </c>
+      <c r="H50" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="I50" s="6" t="n">
+        <v>20</v>
+      </c>
+      <c r="J50" s="9" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="K50" s="9" t="n">
+        <v>28.17</v>
+      </c>
+      <c r="L50" s="6" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="M50" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="N50" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B51" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="C51" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D51" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E51" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F51" s="43" t="n">
+        <v>20</v>
+      </c>
+      <c r="G51" s="44" t="n">
+        <v>538.26</v>
+      </c>
+      <c r="H51" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="I51" s="6" t="n">
+        <v>20</v>
+      </c>
+      <c r="J51" s="9" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="K51" s="9" t="n">
+        <v>10.8</v>
+      </c>
+      <c r="L51" s="6" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="M51" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="N51" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="45" t="s">
+        <v>14</v>
+      </c>
+      <c r="B52" s="45" t="s">
+        <v>82</v>
+      </c>
+      <c r="C52" s="45" t="s">
+        <v>16</v>
+      </c>
+      <c r="D52" s="45" t="s">
+        <v>17</v>
+      </c>
+      <c r="E52" s="45" t="s">
+        <v>27</v>
+      </c>
+      <c r="F52" s="45" t="n">
+        <v>20</v>
+      </c>
+      <c r="G52" s="44" t="n">
+        <v>509.58</v>
+      </c>
+      <c r="H52" s="44" t="s">
+        <v>83</v>
+      </c>
+      <c r="I52" s="45" t="n">
+        <v>20</v>
+      </c>
+      <c r="J52" s="46" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="K52" s="46" t="n">
+        <v>10.16</v>
+      </c>
+      <c r="L52" s="45" t="n">
+        <v>1.53</v>
+      </c>
+      <c r="M52" s="45" t="n">
+        <v>0</v>
+      </c>
+      <c r="N52" s="45" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="B53" s="39" t="s">
+        <v>84</v>
+      </c>
+      <c r="C53" s="39" t="s">
+        <v>16</v>
+      </c>
+      <c r="D53" s="39" t="s">
+        <v>17</v>
+      </c>
+      <c r="E53" s="39" t="s">
+        <v>85</v>
+      </c>
+      <c r="F53" s="39" t="n">
+        <v>25</v>
+      </c>
+      <c r="G53" s="40" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="H53" s="40" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="I53" s="39" t="n">
+        <v>0</v>
+      </c>
+      <c r="J53" s="40" t="n">
+        <v>0</v>
+      </c>
+      <c r="K53" s="40" t="n">
+        <v>0</v>
+      </c>
+      <c r="L53" s="39" t="n">
+        <v>0</v>
+      </c>
+      <c r="M53" s="39" t="n">
+        <v>0</v>
+      </c>
+      <c r="N53" s="39" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="47" t="s">
+        <v>14</v>
+      </c>
+      <c r="B54" s="47" t="s">
+        <v>84</v>
+      </c>
+      <c r="C54" s="47" t="s">
+        <v>16</v>
+      </c>
+      <c r="D54" s="47" t="s">
+        <v>17</v>
+      </c>
+      <c r="E54" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="F54" s="47" t="n">
+        <v>30</v>
+      </c>
+      <c r="G54" s="42" t="n">
+        <v>537.47</v>
+      </c>
+      <c r="H54" s="42" t="s">
+        <v>86</v>
+      </c>
+      <c r="I54" s="47" t="n">
+        <v>20</v>
+      </c>
+      <c r="J54" s="48" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="K54" s="48" t="n">
+        <v>16.08</v>
+      </c>
+      <c r="L54" s="47" t="n">
+        <v>2.43</v>
+      </c>
+      <c r="M54" s="47" t="n">
+        <v>0</v>
+      </c>
+      <c r="N54" s="47" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B55" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="C55" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D55" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E55" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F55" s="10" t="n">
+        <v>30</v>
+      </c>
+      <c r="G55" s="11" t="n">
+        <v>535.66</v>
+      </c>
+      <c r="H55" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="I55" s="6" t="n">
+        <v>20</v>
+      </c>
+      <c r="J55" s="9" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="K55" s="9" t="n">
+        <v>16.11</v>
+      </c>
+      <c r="L55" s="6" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="M55" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="N55" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="B56" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="C56" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="D56" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="E56" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="F56" s="26" t="n">
+        <v>30</v>
+      </c>
+      <c r="G56" s="11" t="n">
         <v>517.4</v>
       </c>
-      <c r="H49" s="38" t="s">
+      <c r="H56" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="I49" s="5" t="n">
-        <v>20</v>
-      </c>
-      <c r="J49" s="38" t="n">
-        <v>3.6</v>
-      </c>
-      <c r="K49" s="38" t="n">
+      <c r="I56" s="26" t="n">
+        <v>20</v>
+      </c>
+      <c r="J56" s="27" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="K56" s="27" t="n">
         <v>15.48</v>
       </c>
-      <c r="L49" s="5" t="n">
+      <c r="L56" s="26" t="n">
         <v>2.34</v>
       </c>
-      <c r="M49" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="N49" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B50" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="C50" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D50" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E50" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="F50" s="5" t="n">
-        <v>40</v>
-      </c>
-      <c r="G50" s="38" t="n">
-        <v>522.86</v>
-      </c>
-      <c r="H50" s="38" t="s">
-        <v>75</v>
-      </c>
-      <c r="I50" s="5" t="n">
-        <v>20</v>
-      </c>
-      <c r="J50" s="38" t="n">
-        <v>3.6</v>
-      </c>
-      <c r="K50" s="38" t="n">
-        <v>20.87</v>
-      </c>
-      <c r="L50" s="5" t="n">
-        <v>3.15</v>
-      </c>
-      <c r="M50" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="N50" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B51" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="C51" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D51" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E51" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="F51" s="5" t="n">
-        <v>30</v>
-      </c>
-      <c r="G51" s="38" t="n">
-        <v>526.71</v>
-      </c>
-      <c r="H51" s="38" t="s">
-        <v>77</v>
-      </c>
-      <c r="I51" s="5" t="n">
-        <v>20</v>
-      </c>
-      <c r="J51" s="38" t="n">
-        <v>3.6</v>
-      </c>
-      <c r="K51" s="38" t="n">
-        <v>15.76</v>
-      </c>
-      <c r="L51" s="5" t="n">
-        <v>2.38</v>
-      </c>
-      <c r="M51" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="N51" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B52" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="C52" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D52" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E52" s="6" t="s">
+      <c r="M56" s="26" t="n">
+        <v>0</v>
+      </c>
+      <c r="N56" s="26" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="47" t="s">
+        <v>14</v>
+      </c>
+      <c r="B57" s="47" t="s">
+        <v>90</v>
+      </c>
+      <c r="C57" s="47" t="s">
+        <v>16</v>
+      </c>
+      <c r="D57" s="47" t="s">
+        <v>17</v>
+      </c>
+      <c r="E57" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="F57" s="47" t="n">
+        <v>20</v>
+      </c>
+      <c r="G57" s="42" t="n">
+        <v>537.82</v>
+      </c>
+      <c r="H57" s="42" t="s">
+        <v>91</v>
+      </c>
+      <c r="I57" s="47" t="n">
+        <v>20</v>
+      </c>
+      <c r="J57" s="48" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="K57" s="48" t="n">
+        <v>10.72</v>
+      </c>
+      <c r="L57" s="47" t="n">
+        <v>1.62</v>
+      </c>
+      <c r="M57" s="47" t="n">
+        <v>0</v>
+      </c>
+      <c r="N57" s="47" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B58" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="C58" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D58" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E58" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="F52" s="41" t="n">
-        <v>50</v>
-      </c>
-      <c r="G52" s="42" t="n">
-        <v>562.34</v>
-      </c>
-      <c r="H52" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="I52" s="6" t="n">
-        <v>20</v>
-      </c>
-      <c r="J52" s="9" t="n">
-        <v>3.6</v>
-      </c>
-      <c r="K52" s="9" t="n">
-        <v>28.17</v>
-      </c>
-      <c r="L52" s="6" t="n">
-        <v>0.03</v>
-      </c>
-      <c r="M52" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="N52" s="6" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B53" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="C53" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D53" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E53" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F53" s="43" t="n">
-        <v>20</v>
-      </c>
-      <c r="G53" s="44" t="n">
-        <v>538.26</v>
-      </c>
-      <c r="H53" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="I53" s="6" t="n">
-        <v>20</v>
-      </c>
-      <c r="J53" s="9" t="n">
-        <v>3.6</v>
-      </c>
-      <c r="K53" s="9" t="n">
-        <v>10.8</v>
-      </c>
-      <c r="L53" s="6" t="n">
+      <c r="F58" s="12" t="n">
+        <v>25</v>
+      </c>
+      <c r="G58" s="13" t="n">
+        <v>530.5</v>
+      </c>
+      <c r="H58" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="I58" s="6" t="n">
+        <v>20</v>
+      </c>
+      <c r="J58" s="9" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="K58" s="9" t="n">
+        <v>13.3</v>
+      </c>
+      <c r="L58" s="6" t="n">
         <v>0.01</v>
       </c>
-      <c r="M53" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="N53" s="6" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="45" t="s">
-        <v>14</v>
-      </c>
-      <c r="B54" s="45" t="s">
-        <v>82</v>
-      </c>
-      <c r="C54" s="45" t="s">
-        <v>16</v>
-      </c>
-      <c r="D54" s="45" t="s">
-        <v>17</v>
-      </c>
-      <c r="E54" s="45" t="s">
-        <v>27</v>
-      </c>
-      <c r="F54" s="45" t="n">
-        <v>20</v>
-      </c>
-      <c r="G54" s="44" t="n">
-        <v>509.58</v>
-      </c>
-      <c r="H54" s="44" t="s">
-        <v>83</v>
-      </c>
-      <c r="I54" s="45" t="n">
-        <v>20</v>
-      </c>
-      <c r="J54" s="46" t="n">
-        <v>3.6</v>
-      </c>
-      <c r="K54" s="46" t="n">
-        <v>10.16</v>
-      </c>
-      <c r="L54" s="45" t="n">
-        <v>1.53</v>
-      </c>
-      <c r="M54" s="45" t="n">
-        <v>0</v>
-      </c>
-      <c r="N54" s="45" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="39" t="s">
-        <v>14</v>
-      </c>
-      <c r="B55" s="39" t="s">
-        <v>84</v>
-      </c>
-      <c r="C55" s="39" t="s">
-        <v>16</v>
-      </c>
-      <c r="D55" s="39" t="s">
-        <v>17</v>
-      </c>
-      <c r="E55" s="39" t="s">
-        <v>85</v>
-      </c>
-      <c r="F55" s="39" t="n">
-        <v>25</v>
-      </c>
-      <c r="G55" s="40" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="H55" s="40" t="n">
-        <v>12.5</v>
-      </c>
-      <c r="I55" s="39" t="n">
-        <v>0</v>
-      </c>
-      <c r="J55" s="40" t="n">
-        <v>0</v>
-      </c>
-      <c r="K55" s="40" t="n">
-        <v>0</v>
-      </c>
-      <c r="L55" s="39" t="n">
-        <v>0</v>
-      </c>
-      <c r="M55" s="39" t="n">
-        <v>0</v>
-      </c>
-      <c r="N55" s="39" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="47" t="s">
-        <v>14</v>
-      </c>
-      <c r="B56" s="47" t="s">
-        <v>84</v>
-      </c>
-      <c r="C56" s="47" t="s">
-        <v>16</v>
-      </c>
-      <c r="D56" s="47" t="s">
-        <v>17</v>
-      </c>
-      <c r="E56" s="47" t="s">
-        <v>27</v>
-      </c>
-      <c r="F56" s="47" t="n">
-        <v>30</v>
-      </c>
-      <c r="G56" s="42" t="n">
-        <v>537.47</v>
-      </c>
-      <c r="H56" s="42" t="s">
-        <v>86</v>
-      </c>
-      <c r="I56" s="47" t="n">
-        <v>20</v>
-      </c>
-      <c r="J56" s="48" t="n">
-        <v>3.6</v>
-      </c>
-      <c r="K56" s="48" t="n">
-        <v>16.08</v>
-      </c>
-      <c r="L56" s="47" t="n">
-        <v>2.43</v>
-      </c>
-      <c r="M56" s="47" t="n">
-        <v>0</v>
-      </c>
-      <c r="N56" s="47" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B57" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="C57" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D57" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E57" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F57" s="10" t="n">
-        <v>30</v>
-      </c>
-      <c r="G57" s="11" t="n">
-        <v>535.66</v>
-      </c>
-      <c r="H57" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="I57" s="6" t="n">
-        <v>20</v>
-      </c>
-      <c r="J57" s="9" t="n">
-        <v>3.6</v>
-      </c>
-      <c r="K57" s="9" t="n">
-        <v>16.11</v>
-      </c>
-      <c r="L57" s="6" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="M57" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="N57" s="6" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="B58" s="26" t="s">
-        <v>89</v>
-      </c>
-      <c r="C58" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="D58" s="26" t="s">
-        <v>17</v>
-      </c>
-      <c r="E58" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="F58" s="26" t="n">
-        <v>30</v>
-      </c>
-      <c r="G58" s="11" t="n">
-        <v>517.4</v>
-      </c>
-      <c r="H58" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="I58" s="26" t="n">
-        <v>20</v>
-      </c>
-      <c r="J58" s="27" t="n">
-        <v>3.6</v>
-      </c>
-      <c r="K58" s="27" t="n">
-        <v>15.48</v>
-      </c>
-      <c r="L58" s="26" t="n">
-        <v>2.34</v>
-      </c>
-      <c r="M58" s="26" t="n">
-        <v>0</v>
-      </c>
-      <c r="N58" s="26" t="n">
+      <c r="M58" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="N58" s="6" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="47" t="s">
-        <v>14</v>
-      </c>
-      <c r="B59" s="47" t="s">
-        <v>90</v>
-      </c>
-      <c r="C59" s="47" t="s">
-        <v>16</v>
-      </c>
-      <c r="D59" s="47" t="s">
-        <v>17</v>
-      </c>
-      <c r="E59" s="47" t="s">
-        <v>27</v>
-      </c>
-      <c r="F59" s="47" t="n">
-        <v>20</v>
-      </c>
-      <c r="G59" s="42" t="n">
-        <v>537.82</v>
-      </c>
-      <c r="H59" s="42" t="s">
-        <v>91</v>
-      </c>
-      <c r="I59" s="47" t="n">
-        <v>20</v>
-      </c>
-      <c r="J59" s="48" t="n">
-        <v>3.6</v>
-      </c>
-      <c r="K59" s="48" t="n">
-        <v>10.72</v>
-      </c>
-      <c r="L59" s="47" t="n">
-        <v>1.62</v>
-      </c>
-      <c r="M59" s="47" t="n">
-        <v>0</v>
-      </c>
-      <c r="N59" s="47" t="n">
+      <c r="A59" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B59" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="C59" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D59" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E59" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="F59" s="15" t="n">
+        <v>8</v>
+      </c>
+      <c r="G59" s="13" t="n">
+        <v>478.86</v>
+      </c>
+      <c r="H59" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="I59" s="15" t="n">
+        <v>6.4</v>
+      </c>
+      <c r="J59" s="49" t="n">
+        <v>1.16</v>
+      </c>
+      <c r="K59" s="49" t="n">
+        <v>3.82</v>
+      </c>
+      <c r="L59" s="15" t="n">
+        <v>0.57</v>
+      </c>
+      <c r="M59" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="N59" s="15" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B60" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="C60" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D60" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E60" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F60" s="12" t="n">
-        <v>25</v>
+      <c r="A60" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B60" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="C60" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D60" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E60" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="F60" s="15" t="n">
+        <v>17</v>
       </c>
       <c r="G60" s="13" t="n">
-        <v>530.5</v>
-      </c>
-      <c r="H60" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="I60" s="6" t="n">
-        <v>20</v>
-      </c>
-      <c r="J60" s="9" t="n">
-        <v>3.6</v>
-      </c>
-      <c r="K60" s="9" t="n">
-        <v>13.3</v>
-      </c>
-      <c r="L60" s="6" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="M60" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="N60" s="6" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="B61" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="C61" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="D61" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="E61" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="F61" s="15" t="n">
-        <v>8</v>
-      </c>
-      <c r="G61" s="13" t="n">
         <v>478.86</v>
       </c>
-      <c r="H61" s="13" t="s">
-        <v>95</v>
-      </c>
-      <c r="I61" s="15" t="n">
-        <v>6.4</v>
-      </c>
-      <c r="J61" s="49" t="n">
-        <v>1.16</v>
-      </c>
-      <c r="K61" s="49" t="n">
-        <v>3.82</v>
-      </c>
-      <c r="L61" s="15" t="n">
-        <v>0.57</v>
-      </c>
-      <c r="M61" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="N61" s="15" t="n">
+      <c r="H60" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="I60" s="15" t="n">
+        <v>13.6</v>
+      </c>
+      <c r="J60" s="49" t="n">
+        <v>2.44</v>
+      </c>
+      <c r="K60" s="49" t="n">
+        <v>8.12</v>
+      </c>
+      <c r="L60" s="15" t="n">
+        <v>1.23</v>
+      </c>
+      <c r="M60" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="N60" s="15" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="B62" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="C62" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="D62" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="E62" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="F62" s="15" t="n">
-        <v>17</v>
-      </c>
-      <c r="G62" s="13" t="n">
-        <v>478.86</v>
-      </c>
-      <c r="H62" s="13" t="s">
-        <v>96</v>
-      </c>
-      <c r="I62" s="15" t="n">
-        <v>13.6</v>
-      </c>
-      <c r="J62" s="49" t="n">
-        <v>2.44</v>
-      </c>
-      <c r="K62" s="49" t="n">
-        <v>8.12</v>
-      </c>
-      <c r="L62" s="15" t="n">
-        <v>1.23</v>
-      </c>
-      <c r="M62" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="N62" s="15" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="5" t="s">
+      <c r="A62" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="B64" s="5"/>
-      <c r="C64" s="5" t="n">
+      <c r="B62" s="5"/>
+      <c r="C62" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="D64" s="5" t="s">
+      <c r="D62" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="E64" s="5" t="n">
+      <c r="E62" s="5" t="n">
         <v>660</v>
       </c>
-      <c r="F64" s="5"/>
-      <c r="G64" s="38"/>
-      <c r="H64" s="38"/>
-      <c r="I64" s="5"/>
-      <c r="J64" s="38"/>
-      <c r="K64" s="38"/>
-      <c r="L64" s="5"/>
-      <c r="M64" s="5"/>
-      <c r="N64" s="5"/>
-    </row>
+      <c r="F62" s="5"/>
+      <c r="G62" s="38"/>
+      <c r="H62" s="38"/>
+      <c r="I62" s="5"/>
+      <c r="J62" s="38"/>
+      <c r="K62" s="38"/>
+      <c r="L62" s="5"/>
+      <c r="M62" s="5"/>
+      <c r="N62" s="5"/>
+    </row>
+    <row r="1048545" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048546" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048547" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048548" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048549" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -3771,7 +3737,7 @@
   </sheetPr>
   <dimension ref="A1:N17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C22" activeCellId="0" sqref="C22"/>
     </sheetView>
   </sheetViews>
@@ -3915,7 +3881,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" s="22" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" s="56" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="22" t="s">
         <v>14</v>
       </c>
@@ -3959,51 +3925,51 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" s="58" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="56" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="56" t="s">
+    <row r="5" s="56" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="57" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="57" t="s">
         <v>55</v>
       </c>
-      <c r="C5" s="56" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="56" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="56" t="s">
-        <v>27</v>
-      </c>
-      <c r="F5" s="56" t="n">
+      <c r="C5" s="57" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="57" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="57" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="57" t="n">
         <v>50</v>
       </c>
-      <c r="G5" s="56" t="n">
+      <c r="G5" s="57" t="n">
         <v>504.97</v>
       </c>
-      <c r="H5" s="57" t="s">
+      <c r="H5" s="58" t="s">
         <v>57</v>
       </c>
-      <c r="I5" s="56" t="n">
-        <v>20</v>
-      </c>
-      <c r="J5" s="56" t="n">
-        <v>3.6</v>
-      </c>
-      <c r="K5" s="56" t="n">
+      <c r="I5" s="57" t="n">
+        <v>20</v>
+      </c>
+      <c r="J5" s="57" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="K5" s="57" t="n">
         <v>25.05</v>
       </c>
-      <c r="L5" s="56" t="n">
+      <c r="L5" s="57" t="n">
         <v>3.81</v>
       </c>
-      <c r="M5" s="56" t="n">
+      <c r="M5" s="57" t="n">
         <v>355</v>
       </c>
-      <c r="N5" s="56" t="n">
+      <c r="N5" s="57" t="n">
         <v>50</v>
       </c>
     </row>
-    <row r="6" s="61" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="59" t="s">
         <v>14</v>
       </c>
@@ -4047,7 +4013,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" s="61" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="59" t="s">
         <v>14</v>
       </c>
@@ -4252,21 +4218,21 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E16" s="58" t="s">
+      <c r="E16" s="57" t="s">
         <v>18</v>
       </c>
-      <c r="F16" s="58" t="n">
+      <c r="F16" s="57" t="n">
         <v>50</v>
       </c>
-      <c r="G16" s="58" t="n">
+      <c r="G16" s="57" t="n">
         <v>517</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E17" s="61" t="s">
+      <c r="E17" s="56" t="s">
         <v>18</v>
       </c>
-      <c r="F17" s="61" t="n">
+      <c r="F17" s="56" t="n">
         <v>60</v>
       </c>
       <c r="G17" s="59" t="n">

</xml_diff>